<commit_message>
removed useless tesseract versions
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i530455/Documents/MLBenchmarking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD737811-B1DB-F846-8508-0A9F9DFD50D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519C0E28-967A-2B4F-8E19-0E47ABFBBF20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="17520" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6800" yWindow="500" windowWidth="14540" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Watermark Tests</t>
   </si>
@@ -45,6 +55,12 @@
   </si>
   <si>
     <t>Tesseract</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
   </si>
 </sst>
 </file>
@@ -60,11 +76,13 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -98,7 +116,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -317,10 +335,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A3:C33"/>
+  <dimension ref="A3:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -446,7 +464,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="4">
-        <v>3.2239999999999998E-2</v>
+        <v>3.2240000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -514,48 +532,58 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>0.98399999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="2">
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <v>5.1109999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="1">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>13.27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="2">
+        <v>13</v>
+      </c>
+      <c r="C31">
+        <v>0.60599999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <f>SUM(C19:C31)/13</f>
+        <v>9.8550000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C28">
-        <v>8.1189999999999998</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="1">
-        <v>10</v>
-      </c>
-      <c r="C29">
-        <v>0.98399999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="2">
-        <v>11</v>
-      </c>
-      <c r="C30">
-        <v>5.1109999999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="1">
-        <v>12</v>
-      </c>
-      <c r="C31">
-        <v>13.27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="2">
-        <v>13</v>
-      </c>
-      <c r="C32">
-        <v>0.60599999999999998</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="1">
-        <v>14</v>
+      <c r="C37">
+        <f>_xlfn.STDEV.P(C19:C31)</f>
+        <v>20.380810408888966</v>
       </c>
     </row>
   </sheetData>

</xml_diff>